<commit_message>
Update all tickers 09-21
</commit_message>
<xml_diff>
--- a/all_tickers_2025.xlsx
+++ b/all_tickers_2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/williampan/Documents/PROJECTS/stocks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{56ED1A96-EB19-4941-97CA-D83C0AA4E8CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D280C63-529D-8A47-ACB1-B6B8F7C629D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14620" yWindow="-24280" windowWidth="28040" windowHeight="17440" xr2:uid="{C117A0A1-24C5-A14E-8C2F-8D0DA643FAE9}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17700" xr2:uid="{C117A0A1-24C5-A14E-8C2F-8D0DA643FAE9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t>Ticker</t>
   </si>
@@ -44,7 +44,157 @@
     <t>NVDA</t>
   </si>
   <si>
-    <t>AAPL</t>
+    <t>CRDO</t>
+  </si>
+  <si>
+    <t>LEU</t>
+  </si>
+  <si>
+    <t>INOD</t>
+  </si>
+  <si>
+    <t>KTOS</t>
+  </si>
+  <si>
+    <t>STRL</t>
+  </si>
+  <si>
+    <t>RMBS</t>
+  </si>
+  <si>
+    <t>IESC</t>
+  </si>
+  <si>
+    <t>IDCC</t>
+  </si>
+  <si>
+    <t>TLN</t>
+  </si>
+  <si>
+    <t>BBW</t>
+  </si>
+  <si>
+    <t>FIX</t>
+  </si>
+  <si>
+    <t>COOP</t>
+  </si>
+  <si>
+    <t>AVGO</t>
+  </si>
+  <si>
+    <t>BELFB</t>
+  </si>
+  <si>
+    <t>PRIM</t>
+  </si>
+  <si>
+    <t>DXPE</t>
+  </si>
+  <si>
+    <t>RIOT</t>
+  </si>
+  <si>
+    <t>REVG</t>
+  </si>
+  <si>
+    <t>HWM</t>
+  </si>
+  <si>
+    <t>AXON</t>
+  </si>
+  <si>
+    <t>RCL</t>
+  </si>
+  <si>
+    <t>VRT</t>
+  </si>
+  <si>
+    <t>NRG</t>
+  </si>
+  <si>
+    <t>VSEC</t>
+  </si>
+  <si>
+    <t>FTAI</t>
+  </si>
+  <si>
+    <t>LMB</t>
+  </si>
+  <si>
+    <t>CECO</t>
+  </si>
+  <si>
+    <t>ROAD</t>
+  </si>
+  <si>
+    <t>GE</t>
+  </si>
+  <si>
+    <t>APH</t>
+  </si>
+  <si>
+    <t>ATGE</t>
+  </si>
+  <si>
+    <t>ANET</t>
+  </si>
+  <si>
+    <t>EME</t>
+  </si>
+  <si>
+    <t>BWXT</t>
+  </si>
+  <si>
+    <t>LAUR</t>
+  </si>
+  <si>
+    <t>LRN</t>
+  </si>
+  <si>
+    <t>FTI</t>
+  </si>
+  <si>
+    <t>USLM</t>
+  </si>
+  <si>
+    <t>CW</t>
+  </si>
+  <si>
+    <t>TKO</t>
+  </si>
+  <si>
+    <t>DRS</t>
+  </si>
+  <si>
+    <t>SNEX</t>
+  </si>
+  <si>
+    <t>ESQ</t>
+  </si>
+  <si>
+    <t>HWKN</t>
+  </si>
+  <si>
+    <t>SGI</t>
+  </si>
+  <si>
+    <t>BLX</t>
+  </si>
+  <si>
+    <t>NBN</t>
+  </si>
+  <si>
+    <t>TBBK</t>
+  </si>
+  <si>
+    <t>EVR</t>
+  </si>
+  <si>
+    <t>NVT</t>
+  </si>
+  <si>
+    <t>MLI</t>
   </si>
 </sst>
 </file>
@@ -80,8 +230,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -416,27 +567,278 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44154919-0342-3440-BCB3-C12778AD65DA}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:B53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="1"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>2</v>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>